<commit_message>
Added more processed plates, added a TT spacer for new handles and added code to design a crossbar for a crisscross square
</commit_message>
<xml_diff>
--- a/core_plates/sw_src002_slatcore.xlsx
+++ b/core_plates/sw_src002_slatcore.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stellawang/Dropbox (HMS)/sequences/platelayouts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Documents/Shih_Lab_Postdoc/research_projects/crisscross_code/core_plates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A593CD-DD49-AD40-8208-D7F53BBD70ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7312DBF-F75C-804A-963B-292EF0D1116F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21640" yWindow="7580" windowWidth="26840" windowHeight="18080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17920" yWindow="500" windowWidth="17920" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Names" sheetId="1" r:id="rId1"/>
@@ -3538,14 +3538,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="Y27" sqref="Y27"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="173" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" style="1" customWidth="1"/>
-    <col min="2" max="25" width="6.33203125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="28.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="25" width="6.33203125" style="1" customWidth="1"/>
     <col min="26" max="26" width="34.6640625" style="1" customWidth="1"/>
     <col min="27" max="27" width="8.83203125" style="1" customWidth="1"/>
     <col min="28" max="16384" width="8.83203125" style="1"/>
@@ -4524,13 +4525,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="228" workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="25" width="8.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="25" width="8.83203125" style="1" customWidth="1"/>
     <col min="26" max="26" width="36.5" style="1" customWidth="1"/>
     <col min="27" max="27" width="8.83203125" style="1" customWidth="1"/>
     <col min="28" max="16384" width="8.83203125" style="1"/>
@@ -5513,7 +5516,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="25" width="8.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="43.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="25" width="8.83203125" style="1" customWidth="1"/>
     <col min="26" max="26" width="31.83203125" style="1" customWidth="1"/>
     <col min="27" max="27" width="8.83203125" style="1" customWidth="1"/>
     <col min="28" max="16384" width="8.83203125" style="1"/>

</xml_diff>